<commit_message>
updates to load data script
</commit_message>
<xml_diff>
--- a/Practice Data/Laura's Data/metadata.xlsx
+++ b/Practice Data/Laura's Data/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ObrienJas\Documents\Students-PostDocs-Terms\Current\Malek Smadi\Data for Malek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ObrienJas\Documents\GitHub\Maleks_qPCR_Pipeline\Practice Data\Laura's Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931EECFE-C3BA-4E75-81F5-8B4E2AA24F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BADE76-4A31-497E-813A-3ACFEB08A452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,21 +44,9 @@
     <t>site</t>
   </si>
   <si>
-    <t>BL-1</t>
-  </si>
-  <si>
-    <t>BL-2</t>
-  </si>
-  <si>
-    <t>BL-3</t>
-  </si>
-  <si>
     <t>blank</t>
   </si>
   <si>
-    <t>BL-4</t>
-  </si>
-  <si>
     <t>wetland_3</t>
   </si>
   <si>
@@ -147,6 +135,18 @@
   </si>
   <si>
     <t>WL8_4</t>
+  </si>
+  <si>
+    <t>BL_1</t>
+  </si>
+  <si>
+    <t>BL_2</t>
+  </si>
+  <si>
+    <t>BL_3</t>
+  </si>
+  <si>
+    <t>BL_4</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,226 +486,226 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Laura (xml -> xlsx) (xlsx -> 2 txt)
</commit_message>
<xml_diff>
--- a/Practice Data/Laura's Data/metadata.xlsx
+++ b/Practice Data/Laura's Data/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ObrienJas\Documents\GitHub\Maleks_qPCR_Pipeline\Practice Data\Laura's Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smadim\Documents\GitHub\Maleks_qPCR_Pipeline\Practice Data\Laura's Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BADE76-4A31-497E-813A-3ACFEB08A452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9ECA2C-EA69-4DD0-8C82-4B8141D11FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
-    <t>sampleID</t>
-  </si>
-  <si>
-    <t>site</t>
-  </si>
-  <si>
     <t>blank</t>
   </si>
   <si>
@@ -147,6 +141,12 @@
   </si>
   <si>
     <t>BL_4</t>
+  </si>
+  <si>
+    <t>SampleID</t>
+  </si>
+  <si>
+    <t>Site</t>
   </si>
 </sst>
 </file>
@@ -467,245 +467,245 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B26" t="s">
         <v>27</v>
       </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
load data and display merged Table
</commit_message>
<xml_diff>
--- a/Practice Data/Laura's Data/metadata.xlsx
+++ b/Practice Data/Laura's Data/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ObrienJas\Documents\GitHub\Maleks_qPCR_Pipeline\Practice Data\Laura's Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7623A21D-8631-4D3B-B94E-AD71EEA6AA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F51112B-1E15-4720-98AA-69E34C60742C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="110">
   <si>
     <t>blank</t>
   </si>
@@ -338,13 +338,37 @@
     <t>Min Ct</t>
   </si>
   <si>
-    <t>FIGURE</t>
-  </si>
-  <si>
     <t>PROCEED TO NORMALIZATION</t>
   </si>
   <si>
     <t>QUALITY CONTROL PAGE</t>
+  </si>
+  <si>
+    <t>Select QC Genes</t>
+  </si>
+  <si>
+    <t>Add another QC Gene</t>
+  </si>
+  <si>
+    <t>QC Gene</t>
+  </si>
+  <si>
+    <t>QC Type</t>
+  </si>
+  <si>
+    <t>QC Types</t>
+  </si>
+  <si>
+    <t>Genomic Contamination</t>
+  </si>
+  <si>
+    <t>PCR positive</t>
+  </si>
+  <si>
+    <t>No Template Control</t>
+  </si>
+  <si>
+    <t>Reverse Transcriptase Control</t>
   </si>
 </sst>
 </file>
@@ -375,7 +399,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,6 +421,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,24 +564,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,7 +1117,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AX29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AX1" sqref="AX1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -9623,14 +9657,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678BB225-E418-442B-BA8E-4F7AC6CE34F9}">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -9691,7 +9727,7 @@
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -9788,11 +9824,8 @@
       <c r="J10" s="4"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-      <c r="M10" s="5" t="s">
-        <v>91</v>
-      </c>
+      <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
@@ -9811,8 +9844,10 @@
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="M11" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="N11" s="16"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
@@ -9851,14 +9886,10 @@
         <v>7</v>
       </c>
       <c r="J13" s="4"/>
-      <c r="K13" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="N13" s="9" t="s">
-        <v>86</v>
-      </c>
+      <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
@@ -9876,11 +9907,13 @@
         <v>12</v>
       </c>
       <c r="J14" s="4"/>
-      <c r="K14" s="5"/>
+      <c r="K14" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
@@ -9902,7 +9935,9 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
+      <c r="N15" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
@@ -9922,9 +9957,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="5" t="s">
-        <v>94</v>
-      </c>
+      <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
@@ -9945,8 +9978,10 @@
       <c r="J17" s="4"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
+      <c r="M17" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="N17" s="16"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
@@ -9991,16 +10026,14 @@
         <v>36</v>
       </c>
       <c r="J19" s="4"/>
-      <c r="K19" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="O19" s="9">
-        <v>35</v>
+        <v>103</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
@@ -10021,11 +10054,17 @@
         <v>92</v>
       </c>
       <c r="J20" s="4"/>
-      <c r="K20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
+      <c r="N20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
@@ -10069,17 +10108,13 @@
         <v>87</v>
       </c>
       <c r="J22" s="4"/>
-      <c r="K22" s="5" t="s">
-        <v>96</v>
-      </c>
+      <c r="K22" s="5"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="O22" s="9">
-        <v>14</v>
-      </c>
+      <c r="M22" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="N22" s="16"/>
+      <c r="O22" s="5"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
@@ -10137,12 +10172,21 @@
       <c r="B25" t="s">
         <v>22</v>
       </c>
+      <c r="F25" t="s">
+        <v>105</v>
+      </c>
       <c r="J25" s="4"/>
-      <c r="K25" s="5"/>
+      <c r="K25" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
+      <c r="N25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="O25" s="9">
+        <v>35</v>
+      </c>
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
@@ -10157,6 +10201,9 @@
       </c>
       <c r="B26" t="s">
         <v>27</v>
+      </c>
+      <c r="F26" t="s">
+        <v>106</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="5"/>
@@ -10179,12 +10226,21 @@
       <c r="B27" t="s">
         <v>27</v>
       </c>
+      <c r="F27" t="s">
+        <v>107</v>
+      </c>
       <c r="J27" s="4"/>
-      <c r="K27" s="5"/>
+      <c r="K27" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
+      <c r="N27" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="O27" s="9">
+        <v>14</v>
+      </c>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
@@ -10199,6 +10255,9 @@
       </c>
       <c r="B28" t="s">
         <v>27</v>
+      </c>
+      <c r="F28" t="s">
+        <v>108</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="5"/>
@@ -10221,24 +10280,27 @@
       <c r="B29" t="s">
         <v>27</v>
       </c>
+      <c r="F29" t="s">
+        <v>109</v>
+      </c>
       <c r="J29" s="4"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="3"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
       <c r="V29" s="6"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J30" s="4"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="4"/>
+      <c r="L30" s="5"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
@@ -10247,13 +10309,13 @@
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
-      <c r="U30" s="6"/>
+      <c r="U30" s="5"/>
       <c r="V30" s="6"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J31" s="4"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="4"/>
+      <c r="L31" s="5"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
@@ -10262,38 +10324,36 @@
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
-      <c r="U31" s="6"/>
+      <c r="U31" s="5"/>
       <c r="V31" s="6"/>
     </row>
     <row r="32" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J32" s="4"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10"/>
-      <c r="S32" s="10"/>
-      <c r="T32" s="10"/>
-      <c r="U32" s="6"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="3"/>
       <c r="V32" s="6"/>
     </row>
     <row r="33" spans="10:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J33" s="4"/>
       <c r="K33" s="5"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="10"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
     </row>
@@ -10503,19 +10563,19 @@
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
       <c r="S47" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T47" s="12"/>
       <c r="U47" s="12"/>
       <c r="V47" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="M32:T43"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N8:N9 N13:N14" xr:uid="{D67C1249-DBDC-48E2-BC19-FF16CBFE3456}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N8:N9 N14:N15 N20" xr:uid="{D67C1249-DBDC-48E2-BC19-FF16CBFE3456}">
       <formula1>$F$18:$F$22</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O20" xr:uid="{DFFA311F-2447-4CC0-8172-441E22B61A08}">
+      <formula1>$F$26:$F$29</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>